<commit_message>
cleaning of classif dataset, creating cvs file with dataset of features and creating file with visualization
</commit_message>
<xml_diff>
--- a/train/classif.xlsx
+++ b/train/classif.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20407"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669687D0-8904-49C5-8828-ECB893B84130}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D45C87-6F0F-4E69-99DA-1C148AB9F052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8370" yWindow="2490" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -85,16 +96,10 @@
     <t>Bombus hortorum</t>
   </si>
   <si>
-    <t>Bombus hortorum x2</t>
-  </si>
-  <si>
     <t>Bombus pascuorum</t>
   </si>
   <si>
     <t>Bombus hortorum &amp; Megachile centuncularis</t>
-  </si>
-  <si>
-    <t>Macropis fulvipes ?</t>
   </si>
   <si>
     <t>Isodontia mexicana</t>
@@ -124,7 +129,7 @@
     <t>Apis mellifera &amp; Megachile centuncularis</t>
   </si>
   <si>
-    <t>Anthidium manicatum (+Apis mellifera)</t>
+    <t>Macropis fulvipes</t>
   </si>
 </sst>
 </file>
@@ -444,17 +449,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="D241" sqref="D241"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.62890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -476,7 +481,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -488,7 +493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
@@ -500,7 +505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -512,7 +517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -524,7 +529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -536,7 +541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -548,7 +553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -560,7 +565,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -572,7 +577,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -584,7 +589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -596,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -608,7 +613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -620,7 +625,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -632,7 +637,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -644,7 +649,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -656,7 +661,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -668,7 +673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -680,7 +685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -692,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -704,7 +709,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -716,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -728,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -740,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -752,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -764,7 +769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -776,7 +781,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -788,7 +793,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -800,7 +805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -812,7 +817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -824,7 +829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -836,7 +841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -845,14 +850,14 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
       <c r="B34" t="s">
         <v>7</v>
       </c>
@@ -860,7 +865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -872,7 +877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -884,7 +889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -896,7 +901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -908,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -920,7 +925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -932,7 +937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -944,7 +949,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -956,7 +961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -968,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -980,7 +985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -992,7 +997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1004,7 +1009,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1016,7 +1021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1028,7 +1033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1040,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1052,7 +1057,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1064,7 +1069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1076,7 +1081,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1088,7 +1093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1100,7 +1105,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1112,7 +1117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1124,7 +1129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1136,7 +1141,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1148,7 +1153,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1160,7 +1165,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1172,7 +1177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1181,10 +1186,10 @@
         <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1196,7 +1201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1208,7 +1213,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1220,7 +1225,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1232,7 +1237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
@@ -1244,7 +1249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
@@ -1256,7 +1261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="1">A67+1</f>
         <v>67</v>
@@ -1268,7 +1273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -1280,7 +1285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1292,7 +1297,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1304,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1316,7 +1321,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1328,7 +1333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -1340,7 +1345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -1352,7 +1357,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1361,10 +1366,10 @@
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -1376,7 +1381,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -1385,10 +1390,10 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -1400,7 +1405,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1412,7 +1417,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -1424,7 +1429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -1436,7 +1441,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -1448,7 +1453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -1460,7 +1465,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -1472,7 +1477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1481,70 +1486,70 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87">
-        <f t="shared" si="1"/>
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>6</v>
-      </c>
-      <c r="C87" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A88">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>6</v>
-      </c>
-      <c r="C88" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89">
-        <f t="shared" si="1"/>
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90">
-        <f t="shared" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
-        <v>6</v>
-      </c>
-      <c r="C91" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -1556,7 +1561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -1568,7 +1573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -1580,7 +1585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -1592,7 +1597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -1604,7 +1609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
@@ -1616,7 +1621,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
@@ -1628,7 +1633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
@@ -1640,7 +1645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
@@ -1652,7 +1657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -1664,7 +1669,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>101</v>
@@ -1676,7 +1681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>102</v>
@@ -1688,7 +1693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>103</v>
@@ -1700,7 +1705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>104</v>
@@ -1712,7 +1717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>105</v>
@@ -1724,7 +1729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>106</v>
@@ -1736,7 +1741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>107</v>
@@ -1748,7 +1753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>108</v>
@@ -1760,7 +1765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>109</v>
@@ -1772,7 +1777,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -1784,7 +1789,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>111</v>
@@ -1796,7 +1801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>112</v>
@@ -1808,7 +1813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>113</v>
@@ -1820,7 +1825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>114</v>
@@ -1832,7 +1837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>115</v>
@@ -1844,7 +1849,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>116</v>
@@ -1856,7 +1861,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>117</v>
@@ -1868,7 +1873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>118</v>
@@ -1880,7 +1885,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>119</v>
@@ -1892,7 +1897,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -1904,7 +1909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>121</v>
@@ -1916,7 +1921,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>122</v>
@@ -1928,7 +1933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>123</v>
@@ -1940,7 +1945,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>124</v>
@@ -1952,7 +1957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>125</v>
@@ -1964,7 +1969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>126</v>
@@ -1976,7 +1981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>127</v>
@@ -1988,7 +1993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>128</v>
@@ -2000,7 +2005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -2012,7 +2017,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -2024,7 +2029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" ref="A132:A157" si="2">A131+1</f>
         <v>131</v>
@@ -2036,7 +2041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="2"/>
         <v>132</v>
@@ -2048,7 +2053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="2"/>
         <v>133</v>
@@ -2060,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" si="2"/>
         <v>134</v>
@@ -2072,7 +2077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>135</v>
@@ -2084,7 +2089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>136</v>
@@ -2096,7 +2101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>137</v>
@@ -2108,7 +2113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>138</v>
@@ -2120,7 +2125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>139</v>
@@ -2129,10 +2134,10 @@
         <v>6</v>
       </c>
       <c r="C140" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -2141,10 +2146,10 @@
         <v>6</v>
       </c>
       <c r="C141" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>141</v>
@@ -2153,10 +2158,10 @@
         <v>6</v>
       </c>
       <c r="C142" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>142</v>
@@ -2165,10 +2170,10 @@
         <v>6</v>
       </c>
       <c r="C143" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>143</v>
@@ -2177,10 +2182,10 @@
         <v>6</v>
       </c>
       <c r="C144" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>144</v>
@@ -2189,10 +2194,10 @@
         <v>6</v>
       </c>
       <c r="C145" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>145</v>
@@ -2201,10 +2206,10 @@
         <v>6</v>
       </c>
       <c r="C146" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>146</v>
@@ -2213,10 +2218,10 @@
         <v>6</v>
       </c>
       <c r="C147" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>147</v>
@@ -2225,10 +2230,10 @@
         <v>6</v>
       </c>
       <c r="C148" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>148</v>
@@ -2237,10 +2242,10 @@
         <v>6</v>
       </c>
       <c r="C149" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>149</v>
@@ -2249,10 +2254,10 @@
         <v>6</v>
       </c>
       <c r="C150" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -2261,10 +2266,10 @@
         <v>6</v>
       </c>
       <c r="C151" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>151</v>
@@ -2273,10 +2278,10 @@
         <v>6</v>
       </c>
       <c r="C152" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>152</v>
@@ -2285,10 +2290,10 @@
         <v>6</v>
       </c>
       <c r="C153" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>153</v>
@@ -2297,10 +2302,10 @@
         <v>6</v>
       </c>
       <c r="C154" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>154</v>
@@ -2309,10 +2314,10 @@
         <v>9</v>
       </c>
       <c r="C155" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>155</v>
@@ -2324,7 +2329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>156</v>
@@ -2333,10 +2338,10 @@
         <v>6</v>
       </c>
       <c r="C157" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -2347,7 +2352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -2369,7 +2374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -2380,7 +2385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -2391,7 +2396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -2402,7 +2407,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -2413,7 +2418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -2424,7 +2429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -2432,10 +2437,10 @@
         <v>7</v>
       </c>
       <c r="C166" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -2443,10 +2448,10 @@
         <v>7</v>
       </c>
       <c r="C167" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -2454,10 +2459,10 @@
         <v>7</v>
       </c>
       <c r="C168" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -2465,10 +2470,10 @@
         <v>6</v>
       </c>
       <c r="C169" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -2476,10 +2481,10 @@
         <v>6</v>
       </c>
       <c r="C170" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -2490,7 +2495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -2501,7 +2506,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -2509,10 +2514,10 @@
         <v>6</v>
       </c>
       <c r="C173" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -2523,7 +2528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -2534,7 +2539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <f>A175+1</f>
         <v>175</v>
@@ -2546,7 +2551,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <f t="shared" ref="A177:A199" si="3">A176+1</f>
         <v>176</v>
@@ -2558,7 +2563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <f t="shared" si="3"/>
         <v>177</v>
@@ -2570,7 +2575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <f t="shared" si="3"/>
         <v>178</v>
@@ -2579,10 +2584,10 @@
         <v>6</v>
       </c>
       <c r="C179" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <f t="shared" si="3"/>
         <v>179</v>
@@ -2594,7 +2599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <f t="shared" si="3"/>
         <v>180</v>
@@ -2603,10 +2608,10 @@
         <v>4</v>
       </c>
       <c r="C181" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <f t="shared" si="3"/>
         <v>181</v>
@@ -2615,10 +2620,10 @@
         <v>7</v>
       </c>
       <c r="C182" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <f t="shared" si="3"/>
         <v>182</v>
@@ -2627,10 +2632,10 @@
         <v>7</v>
       </c>
       <c r="C183" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <f t="shared" si="3"/>
         <v>183</v>
@@ -2639,10 +2644,10 @@
         <v>6</v>
       </c>
       <c r="C184" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <f t="shared" si="3"/>
         <v>184</v>
@@ -2654,7 +2659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <f t="shared" si="3"/>
         <v>185</v>
@@ -2666,7 +2671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <f t="shared" si="3"/>
         <v>186</v>
@@ -2675,10 +2680,10 @@
         <v>6</v>
       </c>
       <c r="C187" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <f t="shared" si="3"/>
         <v>187</v>
@@ -2687,10 +2692,10 @@
         <v>7</v>
       </c>
       <c r="C188" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <f t="shared" si="3"/>
         <v>188</v>
@@ -2702,7 +2707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <f t="shared" si="3"/>
         <v>189</v>
@@ -2714,7 +2719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <f t="shared" si="3"/>
         <v>190</v>
@@ -2726,7 +2731,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <f t="shared" si="3"/>
         <v>191</v>
@@ -2738,7 +2743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <f t="shared" si="3"/>
         <v>192</v>
@@ -2747,10 +2752,10 @@
         <v>8</v>
       </c>
       <c r="C193" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <f t="shared" si="3"/>
         <v>193</v>
@@ -2759,10 +2764,10 @@
         <v>8</v>
       </c>
       <c r="C194" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <f t="shared" si="3"/>
         <v>194</v>
@@ -2774,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <f t="shared" si="3"/>
         <v>195</v>
@@ -2786,7 +2791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <f t="shared" si="3"/>
         <v>196</v>
@@ -2798,7 +2803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <f t="shared" si="3"/>
         <v>197</v>
@@ -2810,7 +2815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <f t="shared" si="3"/>
         <v>198</v>
@@ -2822,7 +2827,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <f>A199+1</f>
         <v>199</v>
@@ -2834,7 +2839,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <f>A200+1</f>
         <v>200</v>
@@ -2843,10 +2848,10 @@
         <v>6</v>
       </c>
       <c r="C201" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202">
         <f t="shared" ref="A202:A244" si="4">A201+1</f>
         <v>201</v>
@@ -2855,10 +2860,10 @@
         <v>6</v>
       </c>
       <c r="C202" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203">
         <f t="shared" si="4"/>
         <v>202</v>
@@ -2867,10 +2872,10 @@
         <v>6</v>
       </c>
       <c r="C203" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204">
         <f t="shared" si="4"/>
         <v>203</v>
@@ -2882,7 +2887,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205">
         <f t="shared" si="4"/>
         <v>204</v>
@@ -2894,7 +2899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206">
         <f t="shared" si="4"/>
         <v>205</v>
@@ -2906,7 +2911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207">
         <f t="shared" si="4"/>
         <v>206</v>
@@ -2918,7 +2923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208">
         <f t="shared" si="4"/>
         <v>207</v>
@@ -2927,10 +2932,10 @@
         <v>8</v>
       </c>
       <c r="C208" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209">
         <f t="shared" si="4"/>
         <v>208</v>
@@ -2939,190 +2944,190 @@
         <v>8</v>
       </c>
       <c r="C209" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <f t="shared" si="4"/>
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>6</v>
+      </c>
+      <c r="C211" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <f t="shared" si="4"/>
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>7</v>
+      </c>
+      <c r="C212" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <f t="shared" si="4"/>
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <f t="shared" si="4"/>
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <f t="shared" si="4"/>
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <f t="shared" si="4"/>
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <f t="shared" si="4"/>
+        <v>216</v>
+      </c>
+      <c r="B217" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <f t="shared" si="4"/>
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>7</v>
+      </c>
+      <c r="C218" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <f t="shared" si="4"/>
+        <v>218</v>
+      </c>
+      <c r="B219" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <f t="shared" si="4"/>
+        <v>219</v>
+      </c>
+      <c r="B220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <f t="shared" si="4"/>
+        <v>220</v>
+      </c>
+      <c r="B221" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <f t="shared" si="4"/>
+        <v>221</v>
+      </c>
+      <c r="B222" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <f t="shared" si="4"/>
+        <v>222</v>
+      </c>
+      <c r="B223" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <f t="shared" si="4"/>
+        <v>223</v>
+      </c>
+      <c r="B224" t="s">
+        <v>7</v>
+      </c>
+      <c r="C224" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A210">
-        <f t="shared" si="4"/>
-        <v>209</v>
-      </c>
-      <c r="B210" t="s">
-        <v>6</v>
-      </c>
-      <c r="C210" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A211">
-        <f t="shared" si="4"/>
-        <v>210</v>
-      </c>
-      <c r="B211" t="s">
-        <v>6</v>
-      </c>
-      <c r="C211" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A212">
-        <f t="shared" si="4"/>
-        <v>211</v>
-      </c>
-      <c r="B212" t="s">
-        <v>7</v>
-      </c>
-      <c r="C212" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A213">
-        <f t="shared" si="4"/>
-        <v>212</v>
-      </c>
-      <c r="B213" t="s">
-        <v>7</v>
-      </c>
-      <c r="C213" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A214">
-        <f t="shared" si="4"/>
-        <v>213</v>
-      </c>
-      <c r="B214" t="s">
-        <v>7</v>
-      </c>
-      <c r="C214" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A215">
-        <f t="shared" si="4"/>
-        <v>214</v>
-      </c>
-      <c r="B215" t="s">
-        <v>6</v>
-      </c>
-      <c r="C215" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A216">
-        <f t="shared" si="4"/>
-        <v>215</v>
-      </c>
-      <c r="B216" t="s">
-        <v>6</v>
-      </c>
-      <c r="C216" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A217">
-        <f t="shared" si="4"/>
-        <v>216</v>
-      </c>
-      <c r="B217" t="s">
-        <v>6</v>
-      </c>
-      <c r="C217" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A218">
-        <f t="shared" si="4"/>
-        <v>217</v>
-      </c>
-      <c r="B218" t="s">
-        <v>7</v>
-      </c>
-      <c r="C218" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A219">
-        <f t="shared" si="4"/>
-        <v>218</v>
-      </c>
-      <c r="B219" t="s">
-        <v>6</v>
-      </c>
-      <c r="C219" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A220">
-        <f t="shared" si="4"/>
-        <v>219</v>
-      </c>
-      <c r="B220" t="s">
-        <v>6</v>
-      </c>
-      <c r="C220" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A221">
-        <f t="shared" si="4"/>
-        <v>220</v>
-      </c>
-      <c r="B221" t="s">
-        <v>6</v>
-      </c>
-      <c r="C221" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A222">
-        <f t="shared" si="4"/>
-        <v>221</v>
-      </c>
-      <c r="B222" t="s">
-        <v>6</v>
-      </c>
-      <c r="C222" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A223">
-        <f t="shared" si="4"/>
-        <v>222</v>
-      </c>
-      <c r="B223" t="s">
-        <v>6</v>
-      </c>
-      <c r="C223" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A224">
-        <f t="shared" si="4"/>
-        <v>223</v>
-      </c>
-      <c r="B224" t="s">
-        <v>7</v>
-      </c>
-      <c r="C224" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225">
         <f t="shared" si="4"/>
         <v>224</v>
@@ -3131,10 +3136,10 @@
         <v>8</v>
       </c>
       <c r="C225" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226">
         <f t="shared" si="4"/>
         <v>225</v>
@@ -3143,106 +3148,106 @@
         <v>8</v>
       </c>
       <c r="C226" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <f t="shared" si="4"/>
+        <v>226</v>
+      </c>
+      <c r="B227" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <f t="shared" si="4"/>
+        <v>227</v>
+      </c>
+      <c r="B228" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <f t="shared" si="4"/>
+        <v>228</v>
+      </c>
+      <c r="B229" t="s">
+        <v>6</v>
+      </c>
+      <c r="C229" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <f t="shared" si="4"/>
+        <v>229</v>
+      </c>
+      <c r="B230" t="s">
+        <v>7</v>
+      </c>
+      <c r="C230" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>6</v>
+      </c>
+      <c r="C231" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <f t="shared" si="4"/>
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>7</v>
+      </c>
+      <c r="C232" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <f t="shared" si="4"/>
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>7</v>
+      </c>
+      <c r="C233" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <f t="shared" si="4"/>
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A227">
-        <f t="shared" si="4"/>
-        <v>226</v>
-      </c>
-      <c r="B227" t="s">
-        <v>6</v>
-      </c>
-      <c r="C227" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A228">
-        <f t="shared" si="4"/>
-        <v>227</v>
-      </c>
-      <c r="B228" t="s">
-        <v>6</v>
-      </c>
-      <c r="C228" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A229">
-        <f t="shared" si="4"/>
-        <v>228</v>
-      </c>
-      <c r="B229" t="s">
-        <v>6</v>
-      </c>
-      <c r="C229" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A230">
-        <f t="shared" si="4"/>
-        <v>229</v>
-      </c>
-      <c r="B230" t="s">
-        <v>7</v>
-      </c>
-      <c r="C230" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A231">
-        <f t="shared" si="4"/>
-        <v>230</v>
-      </c>
-      <c r="B231" t="s">
-        <v>6</v>
-      </c>
-      <c r="C231" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A232">
-        <f t="shared" si="4"/>
-        <v>231</v>
-      </c>
-      <c r="B232" t="s">
-        <v>7</v>
-      </c>
-      <c r="C232" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A233">
-        <f t="shared" si="4"/>
-        <v>232</v>
-      </c>
-      <c r="B233" t="s">
-        <v>7</v>
-      </c>
-      <c r="C233" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A234">
-        <f t="shared" si="4"/>
-        <v>233</v>
-      </c>
-      <c r="B234" t="s">
-        <v>7</v>
-      </c>
-      <c r="C234" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235">
         <f t="shared" si="4"/>
         <v>234</v>
@@ -3251,10 +3256,10 @@
         <v>8</v>
       </c>
       <c r="C235" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236">
         <f t="shared" si="4"/>
         <v>235</v>
@@ -3263,10 +3268,10 @@
         <v>7</v>
       </c>
       <c r="C236" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237">
         <f t="shared" si="4"/>
         <v>236</v>
@@ -3275,10 +3280,10 @@
         <v>8</v>
       </c>
       <c r="C237" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238">
         <f t="shared" si="4"/>
         <v>237</v>
@@ -3287,10 +3292,10 @@
         <v>8</v>
       </c>
       <c r="C238" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239">
         <f t="shared" si="4"/>
         <v>238</v>
@@ -3299,10 +3304,10 @@
         <v>8</v>
       </c>
       <c r="C239" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240">
         <f t="shared" si="4"/>
         <v>239</v>
@@ -3314,7 +3319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <f t="shared" si="4"/>
         <v>240</v>
@@ -3326,7 +3331,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <f t="shared" si="4"/>
         <v>241</v>
@@ -3338,7 +3343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <f t="shared" si="4"/>
         <v>242</v>
@@ -3350,7 +3355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <f t="shared" si="4"/>
         <v>243</v>
@@ -3362,7 +3367,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -3373,7 +3378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -3384,7 +3389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -3395,7 +3400,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -3406,7 +3411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -3417,7 +3422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -3428,7 +3433,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>

</xml_diff>